<commit_message>
Switched to new UI  - Fixed bug in SensorProcessor  - Completed the Configuration View
</commit_message>
<xml_diff>
--- a/Documentation/Sensor.xlsx
+++ b/Documentation/Sensor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khoatran/Documents/Project/blindspotdetection/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khoatran/Documents/AndroidStudioProjects/clinfo/BlindSpotDetection/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11FDA63-D6C8-B145-8D71-97E502A9AFAD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A68E8B-0706-984D-B31B-DAE2E841CBAD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="440" windowWidth="24760" windowHeight="15020" activeTab="2" xr2:uid="{69E93666-412D-1840-B86B-C3BDE6018ED4}"/>
+    <workbookView xWindow="780" yWindow="440" windowWidth="24760" windowHeight="15020" xr2:uid="{69E93666-412D-1840-B86B-C3BDE6018ED4}"/>
   </bookViews>
   <sheets>
     <sheet name="Type of Sensor" sheetId="1" r:id="rId1"/>
@@ -735,7 +735,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -766,6 +766,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF5023"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -779,7 +785,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -801,21 +807,30 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF5023"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1126,7 +1141,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F1EFDFD-7786-F546-9DC6-28E085FE3A91}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1357,7 +1372,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA228B35-CCD6-184B-882A-A310DE467AD9}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -1811,45 +1826,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0B6246C-E949-0144-B290-14F28F490E00}">
   <dimension ref="A2:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H21" sqref="H21"/>
+      <selection pane="topRight" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="29.5" customWidth="1"/>
-    <col min="2" max="2" width="26.1640625" style="13" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="25.83203125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" style="13" customWidth="1"/>
-    <col min="6" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="16.1640625" customWidth="1"/>
+    <col min="2" max="2" width="26.1640625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="22" style="15" customWidth="1"/>
+    <col min="4" max="4" width="25.83203125" style="17" customWidth="1"/>
+    <col min="5" max="5" width="24" style="11" customWidth="1"/>
+    <col min="6" max="6" width="27" style="15" customWidth="1"/>
+    <col min="7" max="7" width="16" style="15" customWidth="1"/>
+    <col min="8" max="8" width="28.33203125" style="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>115</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="15" t="s">
         <v>177</v>
       </c>
     </row>
@@ -1857,25 +1873,25 @@
       <c r="A3" t="s">
         <v>116</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="15" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1883,25 +1899,25 @@
       <c r="A4" t="s">
         <v>117</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="15" t="s">
         <v>178</v>
       </c>
     </row>
@@ -1909,25 +1925,25 @@
       <c r="A5" t="s">
         <v>118</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="15" t="s">
         <v>205</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="15" t="s">
         <v>215</v>
       </c>
     </row>
@@ -1935,19 +1951,19 @@
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="15" t="s">
         <v>185</v>
       </c>
     </row>
@@ -1955,10 +1971,10 @@
       <c r="A7" t="s">
         <v>136</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="17" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1966,25 +1982,25 @@
       <c r="A8" t="s">
         <v>138</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="15" t="s">
         <v>198</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="15" t="s">
         <v>182</v>
       </c>
     </row>
@@ -1992,25 +2008,25 @@
       <c r="A9" t="s">
         <v>55</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="15" t="s">
         <v>199</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="15" t="s">
         <v>199</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="15" t="s">
         <v>207</v>
       </c>
     </row>
@@ -2018,19 +2034,19 @@
       <c r="A10" t="s">
         <v>72</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="15" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2038,13 +2054,13 @@
       <c r="A11" t="s">
         <v>200</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="15" t="s">
         <v>202</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="15" t="s">
         <v>201</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="15" t="s">
         <v>208</v>
       </c>
     </row>
@@ -2052,19 +2068,19 @@
       <c r="A12" t="s">
         <v>124</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="18" t="s">
         <v>210</v>
       </c>
     </row>
@@ -2072,14 +2088,14 @@
       <c r="A13" t="s">
         <v>187</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="F13" t="s">
+      <c r="B13" s="12"/>
+      <c r="F13" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="G13" s="17" t="s">
+      <c r="G13" s="19" t="s">
         <v>194</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="15" t="s">
         <v>214</v>
       </c>
     </row>
@@ -2087,20 +2103,20 @@
       <c r="A14" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="D14" s="12" t="s">
+      <c r="B14" s="12"/>
+      <c r="D14" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="E14" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="E14" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="15" t="s">
         <v>209</v>
       </c>
     </row>
@@ -2108,14 +2124,14 @@
       <c r="A15" t="s">
         <v>180</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="F15" t="s">
+      <c r="B15" s="12"/>
+      <c r="F15" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="15" t="s">
         <v>203</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="15" t="s">
         <v>181</v>
       </c>
     </row>
@@ -2123,11 +2139,11 @@
       <c r="A16" t="s">
         <v>191</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="F16" t="s">
+      <c r="B16" s="12"/>
+      <c r="F16" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="15" t="s">
         <v>204</v>
       </c>
     </row>
@@ -2135,14 +2151,14 @@
       <c r="A17" t="s">
         <v>179</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="F17" t="s">
+      <c r="B17" s="12"/>
+      <c r="F17" s="15" t="s">
         <v>192</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="15" t="s">
         <v>192</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="15" t="s">
         <v>213</v>
       </c>
     </row>
@@ -2150,25 +2166,25 @@
       <c r="A18" t="s">
         <v>126</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="E18" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="15" t="s">
         <v>193</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="15" t="s">
         <v>212</v>
       </c>
     </row>
@@ -2176,19 +2192,19 @@
       <c r="A19" t="s">
         <v>127</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="15" t="s">
         <v>174</v>
       </c>
     </row>
@@ -2196,25 +2212,25 @@
       <c r="A20" t="s">
         <v>132</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="C20" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" s="12" t="s">
+      <c r="C20" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="E20" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="15" t="s">
         <v>196</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="15" t="s">
         <v>211</v>
       </c>
     </row>
@@ -2222,44 +2238,44 @@
       <c r="A21" t="s">
         <v>65</v>
       </c>
-      <c r="B21" s="13">
+      <c r="B21" s="11">
         <v>154.94999999999999</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="15">
         <v>50</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E21" s="11">
         <v>299</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="15" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="E22" s="11" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="17" t="s">
         <v>159</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="E23" s="11" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>